<commit_message>
E5 DQN results and refactoring
</commit_message>
<xml_diff>
--- a/data/results/combined_features_refined/Both_testing.xlsx
+++ b/data/results/combined_features_refined/Both_testing.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Episode</t>
+          <t>Values</t>
         </is>
       </c>
       <c r="C1" s="1" t="n">
@@ -453,59 +453,81 @@
       </c>
       <c r="G1" s="1" t="n">
         <v>5</v>
-      </c>
-      <c r="H1" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="n">
-        <v>10</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Final Value</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>2645071.686008946</v>
+      </c>
+      <c r="D2" t="n">
+        <v>3049452.098302247</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2469548.226738013</v>
+      </c>
+      <c r="F2" t="n">
+        <v>2653360.104686474</v>
+      </c>
+      <c r="G2" t="n">
+        <v>2653245.833758925</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C2" t="n">
-        <v>1678711.129210792</v>
-      </c>
-      <c r="D2" t="n">
-        <v>2324444.204069179</v>
-      </c>
-      <c r="E2" t="n">
-        <v>2510366.43399216</v>
-      </c>
-      <c r="F2" t="n">
-        <v>2762443.876718231</v>
-      </c>
-      <c r="G2" t="n">
-        <v>2045259.733821744</v>
-      </c>
-      <c r="H2" t="n">
-        <v>3089359.880035898</v>
-      </c>
-      <c r="I2" t="n">
-        <v>2742576.571532635</v>
-      </c>
-      <c r="J2" t="n">
-        <v>1877481.627665781</v>
-      </c>
-      <c r="K2" t="n">
-        <v>1452357.627277469</v>
-      </c>
-      <c r="L2" t="n">
-        <v>2439101.018088246</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Annualized Return</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0.3788614333539579</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.4451950695318403</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.3479439652969061</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.3802869612158055</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.3802673280104469</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Sharpe Ratio</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0.730558553332663</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.9740564215860639</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.7671793834188858</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.7279514498061527</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.727610642345788</v>
       </c>
     </row>
   </sheetData>

</xml_diff>